<commit_message>
Update webpage with some additional figures.
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelflynn/Library/CloudStorage/Dropbox/consulting/UNO/cluster-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2D6B06-D398-F444-9801-B1F79042C405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CA585F-8652-2249-9F8C-F5CA6B05A9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{F741E534-208F-1C48-9523-D4E3F0506E67}"/>
   </bookViews>
@@ -476,11 +476,11 @@
         <v>0.4236111111111111</v>
       </c>
       <c r="C5" s="1">
-        <v>0.5</v>
+        <v>0.50694444444444442</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>7.6388888888888895E-2</v>
+        <v>8.3333333333333315E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -513,7 +513,7 @@
       </c>
       <c r="D11" s="1">
         <f>SUM(D2:D9)</f>
-        <v>0.18055555555555561</v>
+        <v>0.18750000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update: Working on principal component analysis approach.
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelflynn/Library/CloudStorage/Dropbox/consulting/UNO/cluster-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CA585F-8652-2249-9F8C-F5CA6B05A9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE482FB-50BC-0646-B6B7-0DC42E2E3BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{F741E534-208F-1C48-9523-D4E3F0506E67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Start</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Research factor analysis and principal components analysis methods. Exploratory coding work to look at viability of these methods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working up website to show updates to clustering procedures. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading more on cluster methods and beginning work on website. </t>
   </si>
 </sst>
 </file>
@@ -409,7 +418,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,7 +464,7 @@
         <v>0.1388888888888889</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D18" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D8" si="0">C3-B3</f>
         <v>3.125E-2</v>
       </c>
     </row>
@@ -470,6 +479,9 @@
         <f t="shared" si="0"/>
         <v>1.736111111111116E-2</v>
       </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
@@ -482,11 +494,23 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333315E-2</v>
       </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.5</v>
+      </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.555555555555558E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -513,7 +537,7 @@
       </c>
       <c r="D11" s="1">
         <f>SUM(D2:D9)</f>
-        <v>0.18750000000000003</v>
+        <v>0.24305555555555561</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add visualiation for groupings.
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelflynn/Library/CloudStorage/Dropbox/consulting/UNO/cluster-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE482FB-50BC-0646-B6B7-0DC42E2E3BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC9A314-462E-8649-BA79-0468374F3FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{F741E534-208F-1C48-9523-D4E3F0506E67}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Start</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t xml:space="preserve">Reading more on cluster methods and beginning work on website. </t>
+  </si>
+  <si>
+    <t>Selecting new variables for principal components analysis and revisting data cleaning portion</t>
+  </si>
+  <si>
+    <t>Coding principal components scores.</t>
+  </si>
+  <si>
+    <t>Generate clusters using PC scores and quantile groupings. Visual inspection of different combinations of variables to see if we can make intuitive sense of the different groupings and combinations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working on a table that will show the the principal component scores across the three key dimensiosn broken down by percentiles. I think we need to break out the demographic into a race and economic dimension, though, as major metro areas like NY are occupying a stange middle ground in the current iteration. I think some things some signs of "weak" economic performance, like unemployment, are working against other more positive indicators, like total population and diversity. </t>
   </si>
 </sst>
 </file>
@@ -418,7 +430,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,7 +476,7 @@
         <v>0.1388888888888889</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D8" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D10" si="0">C3-B3</f>
         <v>3.125E-2</v>
       </c>
     </row>
@@ -503,41 +515,74 @@
         <v>0.44444444444444442</v>
       </c>
       <c r="C6" s="1">
-        <v>0.5</v>
+        <v>0.50902777777777775</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>5.555555555555558E-2</v>
+        <v>6.4583333333333326E-2</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.1388888888888889</v>
+      </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D9" s="1"/>
+      <c r="B9" s="1">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5833333333333282E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1">
-        <f>SUM(D2:D9)</f>
-        <v>0.24305555555555561</v>
+      <c r="B10" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -550,7 +595,13 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D15" s="1"/>
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <f>SUM(D2:D10)</f>
+        <v>0.36041666666666661</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D16" s="1"/>

</xml_diff>

<commit_message>
cleaned up the page and updated to 30 quantiles and 30 clusters. I might be able to go back to a smaller number of quanties if need be.
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelflynn/Library/CloudStorage/Dropbox/consulting/UNO/cluster-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC9A314-462E-8649-BA79-0468374F3FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66F5616-6096-924B-B76D-360315285A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{F741E534-208F-1C48-9523-D4E3F0506E67}"/>
+    <workbookView xWindow="20000" yWindow="500" windowWidth="28800" windowHeight="16540" xr2:uid="{F741E534-208F-1C48-9523-D4E3F0506E67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Start</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Research factor analysis and principal components analysis methods. Exploratory coding work to look at viability of these methods.</t>
   </si>
   <si>
@@ -75,14 +72,38 @@
   </si>
   <si>
     <t xml:space="preserve">Working on a table that will show the the principal component scores across the three key dimensiosn broken down by percentiles. I think we need to break out the demographic into a race and economic dimension, though, as major metro areas like NY are occupying a stange middle ground in the current iteration. I think some things some signs of "weak" economic performance, like unemployment, are working against other more positive indicators, like total population and diversity. </t>
+  </si>
+  <si>
+    <t>Broke the demographic variable out into two dimensions. Tried different cluster techniques on the raw PC scores and percentile PC scores. Tried various visualization techniques to try to show the different dimensions captured by the PC scores.</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Total Billables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="167" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -98,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,13 +127,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4261DF-35E9-4F43-A435-C25285D1BD97}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +475,7 @@
     <col min="5" max="5" width="85.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
         <v>7.9861111111111105E-2</v>
       </c>
@@ -468,7 +504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>0.1076388888888889</v>
       </c>
@@ -476,11 +512,11 @@
         <v>0.1388888888888889</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D10" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D14" si="0">C3-B3</f>
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>0.30208333333333331</v>
       </c>
@@ -492,10 +528,10 @@
         <v>1.736111111111116E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>0.4236111111111111</v>
       </c>
@@ -507,10 +543,10 @@
         <v>8.3333333333333315E-2</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>0.44444444444444442</v>
       </c>
@@ -522,10 +558,10 @@
         <v>6.4583333333333326E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>0.10416666666666667</v>
       </c>
@@ -537,10 +573,10 @@
         <v>3.4722222222222224E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>0.31944444444444448</v>
       </c>
@@ -552,10 +588,10 @@
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>0.35694444444444445</v>
       </c>
@@ -567,10 +603,10 @@
         <v>4.5833333333333282E-2</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>0.45833333333333331</v>
       </c>
@@ -582,35 +618,109 @@
         <v>1.3888888888888951E-2</v>
       </c>
       <c r="E10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.20486111111111113</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8194444444444475E-2</v>
+      </c>
+      <c r="E11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1">
-        <f>SUM(D2:D10)</f>
-        <v>0.36041666666666661</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222265E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5">
+        <f>SUM(D2:D14)</f>
+        <v>0.48888888888888893</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2">
+        <f>D20*24*D21</f>
+        <v>2346.666666666667</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed to Euclidean distance. Also changed to use ntile scores to calculate distance for clustering. Increased clusters to 35 and quantiles to 100.
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelflynn/Library/CloudStorage/Dropbox/consulting/UNO/cluster-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66F5616-6096-924B-B76D-360315285A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6615243-2803-D14B-9D03-5BE233584C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20000" yWindow="500" windowWidth="28800" windowHeight="16540" xr2:uid="{F741E534-208F-1C48-9523-D4E3F0506E67}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16540" xr2:uid="{F741E534-208F-1C48-9523-D4E3F0506E67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Start</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>Total Billables</t>
+  </si>
+  <si>
+    <t>Cleaning and preparing data files for sending to client.</t>
+  </si>
+  <si>
+    <t>Revising the input variables used in the principal components scores and updating groupings and clusters</t>
+  </si>
+  <si>
+    <t>Editing visualizations and adding new figures to explore the distribution of the MSAs across different combinations of the principal component scores and cluster IDs</t>
+  </si>
+  <si>
+    <t>Revising to 35 clusters. Also modifying the quantiles to try to get less strange cluster groupings.</t>
   </si>
 </sst>
 </file>
@@ -91,8 +103,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="#,##0.00;[Red]#,##0.00"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -143,8 +155,8 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -466,7 +478,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,7 +524,7 @@
         <v>0.1388888888888889</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D14" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D16" si="0">C3-B3</f>
         <v>3.125E-2</v>
       </c>
     </row>
@@ -647,6 +659,9 @@
         <f t="shared" si="0"/>
         <v>3.4722222222222265E-2</v>
       </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
@@ -659,6 +674,9 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666685E-2</v>
       </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
@@ -673,14 +691,32 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="B15" s="1">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.4604166666666667</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9861111111111116E-2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <v>0.3888888888888889</v>
+      </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.3888888888888889</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
@@ -700,8 +736,8 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5">
-        <f>SUM(D2:D14)</f>
-        <v>0.48888888888888893</v>
+        <f>SUM(D2:D16)</f>
+        <v>0.12986111111111115</v>
       </c>
       <c r="E20" s="4"/>
     </row>
@@ -719,7 +755,7 @@
       </c>
       <c r="D22" s="2">
         <f>D20*24*D21</f>
-        <v>2346.666666666667</v>
+        <v>623.33333333333348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>